<commit_message>
added Excel Azure Calculations
</commit_message>
<xml_diff>
--- a/KN10/ExportedEstimate.xlsx
+++ b/KN10/ExportedEstimate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TBZ\M346\M346_YaCor\KN10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\y_cor\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B34169F-A668-41B8-879F-293F60A105DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1E575F-B72D-4E64-9923-FD88A233B09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>